<commit_message>
Updated code for TestNG setup and Parallel test execution
</commit_message>
<xml_diff>
--- a/src/main/java/org/framework/adib/selendroidTestApp/testData/Test_Data.xlsx
+++ b/src/main/java/org/framework/adib/selendroidTestApp/testData/Test_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -47,13 +47,17 @@
   </si>
   <si>
     <t>Ruby</t>
+  </si>
+  <si>
+    <t>Used</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,7 +426,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.06806640625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -467,10 +471,13 @@
       <c r="F2" t="b">
         <v>1</v>
       </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Updated Framework with the following: 1. Removed TestNG framework 2. Added dependencies for parallel execution 3. New Sessions.yml and Makefile for parallel execution using Cucumber JVM Parallel plugin 4. Updated Config.properties for identifying emulator/devices properties
</commit_message>
<xml_diff>
--- a/src/main/java/org/framework/adib/selendroidTestApp/testData/Test_Data.xlsx
+++ b/src/main/java/org/framework/adib/selendroidTestApp/testData/Test_Data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A42E33-BAFF-7E45-A773-1AE0920076F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="14800" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New_Registration" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -47,17 +48,13 @@
   </si>
   <si>
     <t>Ruby</t>
-  </si>
-  <si>
-    <t>Used</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +204,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -242,6 +256,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -417,19 +448,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.06806640625" collapsed="false"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -452,7 +483,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -468,18 +499,30 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{CF55E84B-1507-D340-8AC5-E01D6E9045DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>